<commit_message>
system test approved by TL
</commit_message>
<xml_diff>
--- a/SimpCity US19 Test Document (4 Pass 0 Fail).xlsx
+++ b/SimpCity US19 Test Document (4 Pass 0 Fail).xlsx
@@ -5,26 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clari\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3922EFC2-57F2-414C-A7A6-FF5B5C24AAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25660299-F533-4AC4-9871-F4BCE1C6AD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US19 Sprint 5" sheetId="21" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1209,6 +1206,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -1253,18 +1262,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1763,8 +1760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3650B6F3-17B5-4438-BAD0-B3F4312E77F5}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1784,10 +1781,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
-      <c r="B1" s="122" t="s">
+      <c r="B1" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="122"/>
+      <c r="C1" s="107"/>
       <c r="D1" s="41"/>
       <c r="E1" s="39"/>
       <c r="F1" s="43"/>
@@ -1800,24 +1797,24 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38"/>
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="124"/>
+      <c r="C2" s="109"/>
       <c r="D2" s="15"/>
-      <c r="E2" s="123" t="s">
+      <c r="E2" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="124"/>
+      <c r="F2" s="109"/>
       <c r="G2" s="19"/>
-      <c r="H2" s="124" t="s">
+      <c r="H2" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="124"/>
-      <c r="J2" s="123" t="s">
+      <c r="I2" s="109"/>
+      <c r="J2" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="125"/>
+      <c r="K2" s="110"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1936,20 +1933,20 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="107"/>
+      <c r="C7" s="111"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="107" t="s">
+      <c r="E7" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="107"/>
+      <c r="F7" s="111"/>
       <c r="G7" s="24"/>
-      <c r="H7" s="107" t="s">
+      <c r="H7" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="107"/>
+      <c r="I7" s="111"/>
       <c r="J7"/>
       <c r="L7" s="4"/>
     </row>
@@ -1959,7 +1956,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="64" t="s">
@@ -1988,7 +1985,7 @@
         <v>24</v>
       </c>
       <c r="F9" s="63" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G9" s="24"/>
       <c r="H9" s="67" t="s">
@@ -2080,37 +2077,37 @@
       </c>
     </row>
     <row r="14" spans="1:12" s="71" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="111">
+      <c r="A14" s="115">
         <v>1</v>
       </c>
-      <c r="B14" s="113" t="s">
+      <c r="B14" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="115" t="s">
+      <c r="C14" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="117" t="s">
+      <c r="D14" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="118"/>
-      <c r="F14" s="119"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="121"/>
+      <c r="E14" s="122"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="124"/>
+      <c r="H14" s="125"/>
       <c r="I14" s="93"/>
       <c r="J14" s="93"/>
       <c r="K14" s="94"/>
     </row>
     <row r="15" spans="1:12" ht="319.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="112"/>
-      <c r="B15" s="114"/>
-      <c r="C15" s="116"/>
+      <c r="A15" s="116"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="120"/>
       <c r="D15" s="96" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="108" t="s">
+      <c r="F15" s="112" t="s">
         <v>40</v>
       </c>
       <c r="G15" s="97" t="s">
@@ -2141,7 +2138,7 @@
       <c r="E16" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="109"/>
+      <c r="F16" s="113"/>
       <c r="G16" s="98" t="s">
         <v>38</v>
       </c>
@@ -2170,7 +2167,7 @@
       <c r="E17" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="109"/>
+      <c r="F17" s="113"/>
       <c r="G17" s="101" t="s">
         <v>38</v>
       </c>
@@ -2199,7 +2196,7 @@
       <c r="E18" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="110"/>
+      <c r="F18" s="114"/>
       <c r="G18" s="102" t="s">
         <v>38</v>
       </c>
@@ -2292,11 +2289,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="H7:I7"/>
@@ -2306,6 +2298,11 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F15" xr:uid="{5568DE78-B01F-4F1C-B67C-1AE9B94B27C1}">

</xml_diff>